<commit_message>
first commit after installation
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/oglk3_.xlsx
+++ b/Statystyki_2018/Template/oglk3_.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">uzasadnienia K tabela1 </t>
   </si>
@@ -117,33 +117,33 @@
     <t>Kordyka Krystian</t>
   </si>
   <si>
-    <t>Kowalewska Ula</t>
-  </si>
-  <si>
     <t>Kowalewska Ala</t>
   </si>
   <si>
+    <t>Kowalewska-KowalewskaKowalewska Ula</t>
+  </si>
+  <si>
+    <t>Nowak Jan</t>
+  </si>
+  <si>
+    <t>6023.15</t>
+  </si>
+  <si>
+    <t>8023.15</t>
+  </si>
+  <si>
+    <t>Sokołowski Michał</t>
+  </si>
+  <si>
+    <t>trzaskowski tomasz</t>
+  </si>
+  <si>
     <t>uzasadnienia K tabela2</t>
   </si>
   <si>
-    <t>Nowak Jan</t>
-  </si>
-  <si>
-    <t>Sokołowski Michał</t>
-  </si>
-  <si>
-    <t>trzaskowski tomasz</t>
-  </si>
-  <si>
     <t>uzasadnienia K tabela3</t>
   </si>
   <si>
-    <t>6023.15</t>
-  </si>
-  <si>
-    <t>8023.15</t>
-  </si>
-  <si>
     <t>Sędzia</t>
   </si>
   <si>
@@ -204,12 +204,12 @@
     <t>Kordyka 4 Krystian</t>
   </si>
   <si>
-    <t>Kowalewska 6 Ula</t>
-  </si>
-  <si>
     <t>Kowalewska 7 Ala</t>
   </si>
   <si>
+    <t>Kowalewska-KowalewskaKowalewska 6 Ula</t>
+  </si>
+  <si>
     <t>Nowak 1 Jan</t>
   </si>
   <si>
@@ -222,52 +222,49 @@
     <t>Liczba spraw</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>Zastosowanie tymczasowego aresztowania</t>
+  </si>
+  <si>
+    <t>Stan zdrowia</t>
+  </si>
+  <si>
+    <t>Inne przyczyny</t>
+  </si>
+  <si>
+    <t>Ilość spraw przestawionych II Instancji</t>
+  </si>
+  <si>
+    <t>aj aja</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>933</t>
+  </si>
+  <si>
+    <t>Do 2 miesięcy</t>
+  </si>
+  <si>
+    <t>Od 2 do 3 miesięcy</t>
+  </si>
+  <si>
+    <t>Od 3 do 6 miesięcy</t>
+  </si>
+  <si>
+    <t>Od 6 do 9 miesięcy</t>
+  </si>
+  <si>
+    <t>Ponad 9 miesięcy</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>Zastosowanie tymczasowego aresztowania</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Stan zdrowia</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>Inne przyczyny</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Ilość spraw przestawionych II Instancji</t>
-  </si>
-  <si>
-    <t>aj aja</t>
-  </si>
-  <si>
-    <t>933</t>
-  </si>
-  <si>
-    <t>Do 2 miesięcy</t>
-  </si>
-  <si>
-    <t>Od 2 do 3 miesięcy</t>
-  </si>
-  <si>
-    <t>Od 3 do 6 miesięcy</t>
-  </si>
-  <si>
-    <t>Od 6 do 9 miesięcy</t>
-  </si>
-  <si>
-    <t>Ponad 9 miesięcy</t>
-  </si>
-  <si>
-    <t>%</t>
   </si>
   <si>
     <t>Wpływ wniosku</t>
@@ -1036,7 +1033,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CF2175-37C2-44C4-96D3-26B1AB8CAE8E}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:M4"/>
@@ -1244,6 +1241,129 @@
         <v>0</v>
       </c>
       <c r="M7" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="40">
+        <v>2038</v>
+      </c>
+      <c r="C8" s="40">
+        <v>0</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="40">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
+      </c>
+      <c r="L8" s="40">
+        <v>0</v>
+      </c>
+      <c r="M8" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="40">
+        <v>2056</v>
+      </c>
+      <c r="C9" s="40">
+        <v>0</v>
+      </c>
+      <c r="D9" s="40">
+        <v>0</v>
+      </c>
+      <c r="E9" s="40">
+        <v>0</v>
+      </c>
+      <c r="F9" s="40">
+        <v>0</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="40">
+        <v>0</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="40">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="40">
+        <v>0</v>
+      </c>
+      <c r="M9" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="40">
+        <v>0</v>
+      </c>
+      <c r="C10" s="40">
+        <v>0</v>
+      </c>
+      <c r="D10" s="40">
+        <v>0</v>
+      </c>
+      <c r="E10" s="40">
+        <v>0</v>
+      </c>
+      <c r="F10" s="40">
+        <v>0</v>
+      </c>
+      <c r="G10" s="40">
+        <v>0</v>
+      </c>
+      <c r="H10" s="40">
+        <v>0</v>
+      </c>
+      <c r="I10" s="40">
+        <v>0</v>
+      </c>
+      <c r="J10" s="40">
+        <v>0</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
+      </c>
+      <c r="L10" s="40">
+        <v>0</v>
+      </c>
+      <c r="M10" s="40">
         <v>0</v>
       </c>
     </row>
@@ -1279,7 +1399,7 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="39" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>55</v>
@@ -1287,50 +1407,50 @@
     </row>
     <row r="2" ht="15.75">
       <c r="A2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" ht="15.75">
       <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E3" s="28"/>
     </row>
     <row r="4" ht="15.75">
       <c r="A4" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="45" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E4" s="16"/>
     </row>
     <row r="5" ht="15.75">
       <c r="A5" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1339,7 +1459,7 @@
     </row>
     <row r="6" ht="15.75">
       <c r="A6" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1348,7 +1468,7 @@
     </row>
     <row r="7" ht="15.75">
       <c r="A7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="18"/>
@@ -1368,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C488F36-C513-4748-A1F4-758DBA88C352}">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H3"/>
@@ -1384,7 +1504,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
@@ -1412,162 +1532,6 @@
       </c>
       <c r="H3" s="35" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="40">
-        <v>0</v>
-      </c>
-      <c r="C4" s="40">
-        <v>0</v>
-      </c>
-      <c r="D4" s="40">
-        <v>0</v>
-      </c>
-      <c r="E4" s="40">
-        <v>0</v>
-      </c>
-      <c r="F4" s="40">
-        <v>0</v>
-      </c>
-      <c r="G4" s="40">
-        <v>0</v>
-      </c>
-      <c r="H4" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="40">
-        <v>0</v>
-      </c>
-      <c r="C5" s="40">
-        <v>0</v>
-      </c>
-      <c r="D5" s="40">
-        <v>0</v>
-      </c>
-      <c r="E5" s="40">
-        <v>0</v>
-      </c>
-      <c r="F5" s="40">
-        <v>0</v>
-      </c>
-      <c r="G5" s="40">
-        <v>0</v>
-      </c>
-      <c r="H5" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="40">
-        <v>0</v>
-      </c>
-      <c r="C6" s="40">
-        <v>0</v>
-      </c>
-      <c r="D6" s="40">
-        <v>0</v>
-      </c>
-      <c r="E6" s="40">
-        <v>0</v>
-      </c>
-      <c r="F6" s="40">
-        <v>0</v>
-      </c>
-      <c r="G6" s="40">
-        <v>0</v>
-      </c>
-      <c r="H6" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="40">
-        <v>13.213213</v>
-      </c>
-      <c r="C7" s="40">
-        <v>0</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40">
-        <v>0</v>
-      </c>
-      <c r="F7" s="40">
-        <v>0</v>
-      </c>
-      <c r="G7" s="40">
-        <v>0</v>
-      </c>
-      <c r="H7" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="40">
-        <v>18.918918</v>
-      </c>
-      <c r="C8" s="40">
-        <v>0</v>
-      </c>
-      <c r="D8" s="40">
-        <v>0</v>
-      </c>
-      <c r="E8" s="40">
-        <v>0</v>
-      </c>
-      <c r="F8" s="40">
-        <v>0</v>
-      </c>
-      <c r="G8" s="40">
-        <v>0</v>
-      </c>
-      <c r="H8" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="40">
-        <v>0</v>
-      </c>
-      <c r="C9" s="40">
-        <v>0</v>
-      </c>
-      <c r="D9" s="40">
-        <v>0</v>
-      </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <v>0</v>
-      </c>
-      <c r="G9" s="40">
-        <v>0</v>
-      </c>
-      <c r="H9" s="40">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +1547,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39942BA8-134C-4D0F-BACD-172F16F6A530}">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A2:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F3"/>
@@ -1601,150 +1565,30 @@
         <v>23</v>
       </c>
       <c r="B2" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="36" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>75</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31"/>
       <c r="B3" s="31"/>
       <c r="C3" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="E3" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>79</v>
-      </c>
       <c r="F3" s="31"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="40">
-        <v>0</v>
-      </c>
-      <c r="C4" s="40">
-        <v>0</v>
-      </c>
-      <c r="D4" s="40">
-        <v>0</v>
-      </c>
-      <c r="E4" s="40">
-        <v>0</v>
-      </c>
-      <c r="F4" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="40">
-        <v>0</v>
-      </c>
-      <c r="C5" s="40">
-        <v>0</v>
-      </c>
-      <c r="D5" s="40">
-        <v>0</v>
-      </c>
-      <c r="E5" s="40">
-        <v>0</v>
-      </c>
-      <c r="F5" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="40">
-        <v>0</v>
-      </c>
-      <c r="C6" s="40">
-        <v>0</v>
-      </c>
-      <c r="D6" s="40">
-        <v>0</v>
-      </c>
-      <c r="E6" s="40">
-        <v>0</v>
-      </c>
-      <c r="F6" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="40">
-        <v>13.213213</v>
-      </c>
-      <c r="C7" s="40">
-        <v>0</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40">
-        <v>0</v>
-      </c>
-      <c r="F7" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="40">
-        <v>18.918918</v>
-      </c>
-      <c r="C8" s="40">
-        <v>0</v>
-      </c>
-      <c r="D8" s="40">
-        <v>0</v>
-      </c>
-      <c r="E8" s="40">
-        <v>0</v>
-      </c>
-      <c r="F8" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="40">
-        <v>0</v>
-      </c>
-      <c r="C9" s="40">
-        <v>0</v>
-      </c>
-      <c r="D9" s="40">
-        <v>0</v>
-      </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells>
@@ -1777,35 +1621,35 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>81</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
       <c r="G2" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31"/>
       <c r="B3" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="D3" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="E3" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="F3" s="34" t="s">
         <v>86</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>87</v>
       </c>
       <c r="G3" s="38"/>
     </row>
@@ -1883,7 +1727,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="40">
-        <v>0</v>
+        <v>13.213213</v>
       </c>
       <c r="C7" s="40">
         <v>0</v>
@@ -1906,7 +1750,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="40">
-        <v>0</v>
+        <v>18.918918</v>
       </c>
       <c r="C8" s="40">
         <v>0</v>
@@ -1970,7 +1814,7 @@
   <sheetData>
     <row r="1" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" ht="15.75">
@@ -2050,7 +1894,7 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="40">
         <v>0</v>
@@ -2091,7 +1935,7 @@
     </row>
     <row r="6">
       <c r="A6" s="39" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="40">
         <v>0</v>
@@ -2173,7 +2017,7 @@
     </row>
     <row r="8">
       <c r="A8" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="40">
         <v>0</v>
@@ -2214,7 +2058,7 @@
     </row>
     <row r="9">
       <c r="A9" s="39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="40">
         <v>0</v>
@@ -2255,7 +2099,7 @@
     </row>
     <row r="10">
       <c r="A10" s="39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="40">
         <v>0</v>
@@ -2321,7 +2165,7 @@
   <sheetData>
     <row r="1" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.75">
@@ -2524,31 +2368,31 @@
     </row>
     <row r="8">
       <c r="A8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="40">
+        <v>0</v>
+      </c>
+      <c r="C8" s="40">
+        <v>0</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0</v>
+      </c>
+      <c r="G8" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="40">
-        <v>0</v>
-      </c>
-      <c r="C8" s="40">
-        <v>0</v>
-      </c>
-      <c r="D8" s="40">
-        <v>0</v>
-      </c>
-      <c r="E8" s="40">
-        <v>0</v>
-      </c>
-      <c r="F8" s="40">
-        <v>0</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" s="40">
         <v>0</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J8" s="40">
         <v>0</v>
@@ -2565,31 +2409,31 @@
     </row>
     <row r="9">
       <c r="A9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="40">
+        <v>0</v>
+      </c>
+      <c r="C9" s="40">
+        <v>0</v>
+      </c>
+      <c r="D9" s="40">
+        <v>0</v>
+      </c>
+      <c r="E9" s="40">
+        <v>0</v>
+      </c>
+      <c r="F9" s="40">
+        <v>0</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="40">
+        <v>0</v>
+      </c>
+      <c r="I9" s="40" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="40">
-        <v>0</v>
-      </c>
-      <c r="C9" s="40">
-        <v>0</v>
-      </c>
-      <c r="D9" s="40">
-        <v>0</v>
-      </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <v>0</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="40">
-        <v>0</v>
-      </c>
-      <c r="I9" s="40" t="s">
-        <v>22</v>
       </c>
       <c r="J9" s="40">
         <v>0</v>
@@ -2606,7 +2450,7 @@
     </row>
     <row r="10">
       <c r="A10" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="40">
         <v>0</v>
@@ -2874,7 +2718,7 @@
     </row>
     <row r="7">
       <c r="A7" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="40">
         <v>2</v>
@@ -2918,7 +2762,7 @@
     </row>
     <row r="8">
       <c r="A8" s="39" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="40">
         <v>3</v>
@@ -2962,7 +2806,7 @@
     </row>
     <row r="9">
       <c r="A9" s="39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="40">
         <v>0</v>
@@ -3370,7 +3214,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="40">
-        <v>0</v>
+        <v>8038</v>
       </c>
       <c r="C6" s="40">
         <v>0</v>
@@ -3393,7 +3237,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="40">
-        <v>0</v>
+        <v>8056</v>
       </c>
       <c r="C7" s="40">
         <v>0</v>
@@ -3471,25 +3315,25 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" ht="16.5">
       <c r="A4" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="43" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" ht="16.5">
       <c r="A5" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="43" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" ht="16.5">
@@ -3518,17 +3362,17 @@
     <row r="1" ht="15.75"/>
     <row r="2" ht="16.5">
       <c r="A2" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" s="44" t="s">
         <v>55</v>
@@ -3557,23 +3401,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="27"/>
       <c r="H3" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3" s="27"/>
       <c r="J3" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K3" s="27"/>
     </row>
@@ -3583,31 +3427,31 @@
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" ht="16.5">

</xml_diff>